<commit_message>
updating files for open data
</commit_message>
<xml_diff>
--- a/data/2024AZMP/AZMP_fall2024_eDNA_isotopes.xlsx
+++ b/data/2024AZMP/AZMP_fall2024_eDNA_isotopes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Science\CESD\HES_MPAGroup\Data\eDNA\2024 AZMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JEFFERYN\Documents\GitHub\eDNA-for-MPAs\data\2024AZMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2866691-F7D5-4D57-9EC8-724949829CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3F716C-528A-482B-8487-F922598498C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15720" xr2:uid="{5C066E4E-7B07-4E8F-BB5A-3D22F55F2FD9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5C066E4E-7B07-4E8F-BB5A-3D22F55F2FD9}"/>
   </bookViews>
   <sheets>
     <sheet name="eDNA_AZMP_fall2024" sheetId="1" r:id="rId1"/>
@@ -1003,9 +1003,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1043,7 +1043,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1149,7 +1149,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1291,7 +1291,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1302,10 +1302,10 @@
   <dimension ref="A1:U69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U9" sqref="U9"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2605,13 +2605,13 @@
         <v>125</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="I21" s="27" t="s">
-        <v>193</v>
+        <v>117</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>119</v>
       </c>
       <c r="J21" s="27" t="s">
         <v>193</v>
@@ -2670,13 +2670,13 @@
         <v>125</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="H22" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="I22" s="27" t="s">
-        <v>193</v>
+        <v>117</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>119</v>
       </c>
       <c r="J22" s="27" t="s">
         <v>193</v>

</xml_diff>